<commit_message>
6-5-2025 08:30 . JCSantos -
</commit_message>
<xml_diff>
--- a/Extra/libros_innarsa@gmail.com.xlsx
+++ b/Extra/libros_innarsa@gmail.com.xlsx
@@ -26,42 +26,42 @@
   </x:si>
   <x:si>
     <x:t xml:space="preserve">
-                        Enigmas. Detectives a domicilio 8. Arte, chanchullos y artimañas
+                        El Cantar de Liébana
                     </x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">
-                        Martin, Paul
+                        Peridis
                                             </x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">978-84-129217-6-2 </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">
-                        Marienbad eléctrico
+    <x:t xml:space="preserve">978-84-670-7234-1 </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+                        La hija de la novicia
                     </x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">
-                        Vila-Matas, Enrique
+                        Álvarez, Elena
                                             </x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">978-84-322-2578-9 </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">
-                        Paraíso Bacuta
+    <x:t xml:space="preserve">978-84-01-03548-7 </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+                        El salón dorado
                     </x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">
-                        Domínguez Rodríguez, Mar
+                        Corral, José Luis
                                             </x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">978-84-608-9409-4 </x:t>
+    <x:t xml:space="preserve">978-84-1314-409-2 </x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>